<commit_message>
updated the original files
</commit_message>
<xml_diff>
--- a/Data/Book_data.xlsx
+++ b/Data/Book_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/76b51dfa0b89278a/CUNY/DATA 607/DATA 607/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{56E93DED-48C8-49B9-A2D1-13B0A747FE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8F37245-9ACC-4A40-91A5-A34D6534FA96}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{56E93DED-48C8-49B9-A2D1-13B0A747FE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02B5627B-4AAC-4D2B-83C8-0653D837A718}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{8E015F56-9D5B-4636-8D0A-5CB1CBA7DA43}"/>
+    <workbookView xWindow="7380" yWindow="0" windowWidth="15660" windowHeight="11112" xr2:uid="{8E015F56-9D5B-4636-8D0A-5CB1CBA7DA43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Title</t>
   </si>
@@ -131,6 +131,15 @@
   </si>
   <si>
     <t>https://www.amazon.com/Build-Life-You-Want-Science/dp/B0C4V8H4CX/ref=sr_1_1?adgrpid=1341405920979738&amp;dib=eyJ2IjoiMSJ9.mYk9YLJBaYAovE3l_RqnvGBfYJ_-B1eU7rIPHoZnZDvpQj3QiT9GqOvr-7A2Fl4SMrp2CLt-0dFZ0wdTDjC5dmqgk3PlNcN054nkY86sWfQw6-HVe2Fsst1YXGah_LrNx1uXsSZ4DixJtgDsjY7MWgzuZiMgAhN5w-RC8AD5_k9VaNAZj2W0qbG9zV1unoYz1IwBi4vtaGc2oWtZU8d_SuSHpG4c20Zc5SrruUOvYT8.zJ0e9PPzZ092MCfNKh5CpumVFwtj5-VDtcnO9lnweYE&amp;dib_tag=se&amp;hvadid=83838162412965&amp;hvbmt=be&amp;hvdev=c&amp;hvlocphy=83184&amp;hvnetw=o&amp;hvqmt=e&amp;hvtargid=kwd-83838936152538%3Aloc-190&amp;hydadcr=14840_13473344&amp;keywords=build+the+life+you+want&amp;qid=1710016091&amp;sr=8-1</t>
+  </si>
+  <si>
+    <t>1-Sep-12</t>
+  </si>
+  <si>
+    <t>20-Nov-15</t>
+  </si>
+  <si>
+    <t>12-Sep-23</t>
   </si>
 </sst>
 </file>
@@ -177,11 +186,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -198,6 +207,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4389B0DC-9CBF-4D75-B2A8-7616BE838F91}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,8 +583,8 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
-        <v>45181</v>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -585,7 +598,7 @@
       <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I2" t="s">
@@ -599,8 +612,8 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
-        <v>42328</v>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -614,10 +627,10 @@
       <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -628,8 +641,8 @@
       <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1">
-        <v>40909</v>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -643,10 +656,10 @@
       <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>